<commit_message>
Add one more session for denfis full recon
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/SaFIN(FRIE)_HFS_Classification_Results.xlsx
+++ b/Experiment_Resulsts/SaFIN(FRIE)_HFS_Classification_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htetnaing/Development/htet_predict_bank_failure/Experiment_Resulsts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E3C3F4-E14F-074B-8EAE-D095550A3E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB6F649-E497-0E4F-8409-0393A3E61F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32320" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{59BFD352-3181-4B2E-9A02-E25DF6E8A988}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="60">
   <si>
     <t>Now</t>
   </si>
@@ -206,10 +206,13 @@
     <t>Increased_Recon</t>
   </si>
   <si>
-    <t>Full_Recon</t>
+    <t>`</t>
   </si>
   <si>
-    <t>`</t>
+    <t>Full_Recon_Anfis</t>
+  </si>
+  <si>
+    <t>Full_Recon_Denfis</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1368,7 @@
         <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J18" t="s">
         <v>32</v>
@@ -3150,10 +3153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D07C55-6007-C646-9152-6264139E81A7}">
-  <dimension ref="A1:AB32"/>
+  <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3162,9 +3165,10 @@
     <col min="12" max="12" width="14.83203125" customWidth="1"/>
     <col min="20" max="20" width="11.5" style="37"/>
     <col min="21" max="21" width="11.5" style="21"/>
+    <col min="30" max="30" width="11.5" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -3172,10 +3176,13 @@
         <v>56</v>
       </c>
       <c r="V1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="21" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>54</v>
       </c>
@@ -3213,8 +3220,20 @@
       <c r="AB2" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF2" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK2" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL2" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -3255,8 +3274,20 @@
       <c r="AB3" s="19">
         <v>3624</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ3" s="19">
+        <v>690</v>
+      </c>
+      <c r="AK3">
+        <v>2934</v>
+      </c>
+      <c r="AL3" s="19">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
         <v>13</v>
       </c>
@@ -3312,8 +3343,26 @@
       <c r="AB4" s="32" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AG4" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI4" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ4" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL4" s="32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3377,8 +3426,29 @@
       <c r="AB5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG5">
+        <v>20.11</v>
+      </c>
+      <c r="AH5">
+        <v>5.41</v>
+      </c>
+      <c r="AI5">
+        <v>15.04</v>
+      </c>
+      <c r="AJ5">
+        <v>84.96</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3442,8 +3512,29 @@
       <c r="AB6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG6">
+        <v>22.46</v>
+      </c>
+      <c r="AH6">
+        <v>4.13</v>
+      </c>
+      <c r="AI6">
+        <v>16.12</v>
+      </c>
+      <c r="AJ6">
+        <v>83.88</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AL6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3507,8 +3598,29 @@
       <c r="AB7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG7">
+        <v>25.36</v>
+      </c>
+      <c r="AH7">
+        <v>5.88</v>
+      </c>
+      <c r="AI7">
+        <v>20.23</v>
+      </c>
+      <c r="AJ7">
+        <v>79.77</v>
+      </c>
+      <c r="AK7">
+        <v>2</v>
+      </c>
+      <c r="AL7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3572,8 +3684,29 @@
       <c r="AB8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG8">
+        <v>18.3</v>
+      </c>
+      <c r="AH8">
+        <v>5.2</v>
+      </c>
+      <c r="AI8">
+        <v>13.62</v>
+      </c>
+      <c r="AJ8">
+        <v>86.38</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3637,8 +3770,29 @@
       <c r="AB9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG9">
+        <v>5.8</v>
+      </c>
+      <c r="AH9">
+        <v>75.290000000000006</v>
+      </c>
+      <c r="AI9">
+        <v>44.65</v>
+      </c>
+      <c r="AJ9">
+        <v>55.35</v>
+      </c>
+      <c r="AK9">
+        <v>3</v>
+      </c>
+      <c r="AL9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -3720,8 +3874,35 @@
         <f t="shared" si="2"/>
         <v>8.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG10" s="5">
+        <f t="shared" ref="AG10:AL10" si="3">AVERAGE(AG5:AG9)</f>
+        <v>18.405999999999999</v>
+      </c>
+      <c r="AH10" s="5">
+        <f t="shared" si="3"/>
+        <v>19.181999999999999</v>
+      </c>
+      <c r="AI10" s="5">
+        <f t="shared" si="3"/>
+        <v>21.931999999999999</v>
+      </c>
+      <c r="AJ10" s="5">
+        <f t="shared" si="3"/>
+        <v>78.067999999999998</v>
+      </c>
+      <c r="AK10" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6</v>
+      </c>
+      <c r="AL10" s="5">
+        <f t="shared" si="3"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -3747,8 +3928,15 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
-    </row>
-    <row r="12" spans="1:28" ht="21" x14ac:dyDescent="0.25">
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="16"/>
+      <c r="AH11" s="16"/>
+      <c r="AI11" s="16"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="16"/>
+    </row>
+    <row r="12" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>54</v>
       </c>
@@ -3774,8 +3962,14 @@
       <c r="Z12" s="32"/>
       <c r="AA12" s="32"/>
       <c r="AB12" s="32"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF12" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ12" s="32"/>
+      <c r="AK12" s="32"/>
+      <c r="AL12" s="32"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="E13" s="32" t="s">
         <v>49</v>
@@ -3811,8 +4005,18 @@
       <c r="AB13" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF13" s="2"/>
+      <c r="AJ13" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK13" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL13" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -3864,8 +4068,23 @@
       <c r="AB14" s="34">
         <v>3620</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="32"/>
+      <c r="AJ14" s="34">
+        <v>686</v>
+      </c>
+      <c r="AK14" s="34">
+        <v>2934</v>
+      </c>
+      <c r="AL14" s="34">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="s">
         <v>13</v>
       </c>
@@ -3925,8 +4144,26 @@
       <c r="AB15" s="32" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AG15" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI15" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ15" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL15" s="32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3993,8 +4230,29 @@
       <c r="AB16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG16">
+        <v>21.49</v>
+      </c>
+      <c r="AH16">
+        <v>9.42</v>
+      </c>
+      <c r="AI16">
+        <v>16.940000000000001</v>
+      </c>
+      <c r="AJ16">
+        <v>83.06</v>
+      </c>
+      <c r="AK16">
+        <v>2</v>
+      </c>
+      <c r="AL16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -4061,8 +4319,29 @@
       <c r="AB17">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG17">
+        <v>22.63</v>
+      </c>
+      <c r="AH17">
+        <v>11.41</v>
+      </c>
+      <c r="AI17">
+        <v>20.07</v>
+      </c>
+      <c r="AJ17">
+        <v>79.930000000000007</v>
+      </c>
+      <c r="AK17">
+        <v>1</v>
+      </c>
+      <c r="AL17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -4129,8 +4408,29 @@
       <c r="AB18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF18" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG18">
+        <v>24.95</v>
+      </c>
+      <c r="AH18">
+        <v>10.23</v>
+      </c>
+      <c r="AI18">
+        <v>19.36</v>
+      </c>
+      <c r="AJ18">
+        <v>80.64</v>
+      </c>
+      <c r="AK18">
+        <v>2</v>
+      </c>
+      <c r="AL18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -4197,8 +4497,29 @@
       <c r="AB19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF19" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG19">
+        <v>23.86</v>
+      </c>
+      <c r="AH19">
+        <v>10.65</v>
+      </c>
+      <c r="AI19">
+        <v>19.88</v>
+      </c>
+      <c r="AJ19">
+        <v>80.12</v>
+      </c>
+      <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AL19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>8</v>
       </c>
@@ -4266,33 +4587,54 @@
       <c r="AB20" s="21">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF20" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG20" s="21">
+        <v>24.04</v>
+      </c>
+      <c r="AH20" s="21">
+        <v>11.25</v>
+      </c>
+      <c r="AI20" s="21">
+        <v>20.22</v>
+      </c>
+      <c r="AJ20" s="21">
+        <v>79.78</v>
+      </c>
+      <c r="AK20" s="21">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="5">
-        <f t="shared" ref="B21:G21" si="3">AVERAGE(B16:B20)</f>
+        <f t="shared" ref="B21:G21" si="4">AVERAGE(B16:B20)</f>
         <v>29.128000000000004</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.9740000000000002</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.417999999999999</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77.582000000000008</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.2</v>
       </c>
       <c r="J21" t="s">
@@ -4302,27 +4644,27 @@
         <v>9</v>
       </c>
       <c r="M21" s="5">
-        <f t="shared" ref="M21:R21" si="4">AVERAGE(M16:M20)</f>
+        <f t="shared" ref="M21:R21" si="5">AVERAGE(M16:M20)</f>
         <v>25.224</v>
       </c>
       <c r="N21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10.802</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.577999999999999</v>
       </c>
       <c r="P21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79.421999999999997</v>
       </c>
       <c r="Q21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2</v>
       </c>
       <c r="R21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.2</v>
       </c>
       <c r="S21" s="3"/>
@@ -4330,31 +4672,58 @@
         <v>9</v>
       </c>
       <c r="W21" s="5">
-        <f t="shared" ref="W21" si="5">AVERAGE(W16:W20)</f>
+        <f t="shared" ref="W21" si="6">AVERAGE(W16:W20)</f>
         <v>23.393999999999998</v>
       </c>
       <c r="X21" s="5">
-        <f t="shared" ref="X21" si="6">AVERAGE(X16:X20)</f>
+        <f t="shared" ref="X21" si="7">AVERAGE(X16:X20)</f>
         <v>10.592000000000001</v>
       </c>
       <c r="Y21" s="5">
-        <f t="shared" ref="Y21" si="7">AVERAGE(Y16:Y20)</f>
+        <f t="shared" ref="Y21" si="8">AVERAGE(Y16:Y20)</f>
         <v>19.294</v>
       </c>
       <c r="Z21" s="5">
-        <f t="shared" ref="Z21" si="8">AVERAGE(Z16:Z20)</f>
+        <f t="shared" ref="Z21" si="9">AVERAGE(Z16:Z20)</f>
         <v>80.705999999999989</v>
       </c>
       <c r="AA21" s="5">
-        <f t="shared" ref="AA21" si="9">AVERAGE(AA16:AA20)</f>
+        <f t="shared" ref="AA21" si="10">AVERAGE(AA16:AA20)</f>
         <v>1.4</v>
       </c>
       <c r="AB21" s="5">
-        <f t="shared" ref="AB21" si="10">AVERAGE(AB16:AB20)</f>
+        <f t="shared" ref="AB21" si="11">AVERAGE(AB16:AB20)</f>
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG21" s="5">
+        <f t="shared" ref="AG21:AL21" si="12">AVERAGE(AG16:AG20)</f>
+        <v>23.393999999999998</v>
+      </c>
+      <c r="AH21" s="5">
+        <f t="shared" si="12"/>
+        <v>10.592000000000001</v>
+      </c>
+      <c r="AI21" s="5">
+        <f t="shared" si="12"/>
+        <v>19.294</v>
+      </c>
+      <c r="AJ21" s="5">
+        <f t="shared" si="12"/>
+        <v>80.705999999999989</v>
+      </c>
+      <c r="AK21" s="5">
+        <f t="shared" si="12"/>
+        <v>1.4</v>
+      </c>
+      <c r="AL21" s="5">
+        <f t="shared" si="12"/>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="E22" s="19"/>
       <c r="G22" s="19"/>
@@ -4369,8 +4738,11 @@
       <c r="V22" s="2"/>
       <c r="Z22" s="19"/>
       <c r="AB22" s="19"/>
-    </row>
-    <row r="23" spans="1:28" ht="21" x14ac:dyDescent="0.25">
+      <c r="AF22" s="2"/>
+      <c r="AJ22" s="19"/>
+      <c r="AL22" s="19"/>
+    </row>
+    <row r="23" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>54</v>
       </c>
@@ -4406,8 +4778,15 @@
       <c r="Z23" s="16"/>
       <c r="AA23" s="16"/>
       <c r="AB23" s="16"/>
-    </row>
-    <row r="24" spans="1:28" ht="21" x14ac:dyDescent="0.25">
+      <c r="AF23" s="16"/>
+      <c r="AG23" s="16"/>
+      <c r="AH23" s="16"/>
+      <c r="AI23" s="16"/>
+      <c r="AJ23" s="16"/>
+      <c r="AK23" s="16"/>
+      <c r="AL23" s="16"/>
+    </row>
+    <row r="24" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -4449,8 +4828,20 @@
       <c r="AB24" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF24" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ24" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK24" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL24" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="s">
         <v>13</v>
       </c>
@@ -4503,8 +4894,23 @@
       <c r="AB25" s="34">
         <v>3604</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG25" s="32"/>
+      <c r="AH25" s="32"/>
+      <c r="AI25" s="32"/>
+      <c r="AJ25" s="34">
+        <v>670</v>
+      </c>
+      <c r="AK25" s="34">
+        <v>2934</v>
+      </c>
+      <c r="AL25" s="34">
+        <v>3604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -4563,8 +4969,26 @@
       <c r="AB26" s="32" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AG26" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH26" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI26" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ26" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK26" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL26" s="32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -4628,8 +5052,29 @@
       <c r="AB27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF27" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG27">
+        <v>28.36</v>
+      </c>
+      <c r="AH27">
+        <v>17.21</v>
+      </c>
+      <c r="AI27">
+        <v>23.58</v>
+      </c>
+      <c r="AJ27">
+        <v>76.42</v>
+      </c>
+      <c r="AK27">
+        <v>1</v>
+      </c>
+      <c r="AL27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -4693,8 +5138,29 @@
       <c r="AB28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG28">
+        <v>31.34</v>
+      </c>
+      <c r="AH28">
+        <v>11.55</v>
+      </c>
+      <c r="AI28">
+        <v>25.09</v>
+      </c>
+      <c r="AJ28">
+        <v>74.91</v>
+      </c>
+      <c r="AK28">
+        <v>1</v>
+      </c>
+      <c r="AL28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -4758,8 +5224,29 @@
       <c r="AB29">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF29" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG29">
+        <v>31.34</v>
+      </c>
+      <c r="AH29">
+        <v>10.14</v>
+      </c>
+      <c r="AI29">
+        <v>25.22</v>
+      </c>
+      <c r="AJ29">
+        <v>74.78</v>
+      </c>
+      <c r="AK29">
+        <v>1</v>
+      </c>
+      <c r="AL29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>8</v>
       </c>
@@ -4823,33 +5310,54 @@
       <c r="AB30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AF30" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG30">
+        <v>36.01</v>
+      </c>
+      <c r="AH30">
+        <v>10.44</v>
+      </c>
+      <c r="AI30">
+        <v>28.45</v>
+      </c>
+      <c r="AJ30">
+        <v>71.55</v>
+      </c>
+      <c r="AK30">
+        <v>1</v>
+      </c>
+      <c r="AL30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="5">
-        <f t="shared" ref="B31:G31" si="11">AVERAGE(B26:B30)</f>
+        <f t="shared" ref="B31:G31" si="13">AVERAGE(B26:B30)</f>
         <v>42.160000000000004</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.9559999999999995</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31.639999999999997</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>68.359999999999985</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.2</v>
       </c>
       <c r="L31" s="20" t="s">
@@ -4895,8 +5403,29 @@
       <c r="AB31" s="21">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" ht="21" x14ac:dyDescent="0.25">
+      <c r="AF31" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG31" s="21">
+        <v>44.22</v>
+      </c>
+      <c r="AH31" s="21">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="AI31" s="21">
+        <v>33.17</v>
+      </c>
+      <c r="AJ31" s="21">
+        <v>66.83</v>
+      </c>
+      <c r="AK31" s="21">
+        <v>1</v>
+      </c>
+      <c r="AL31" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32"/>
@@ -4905,27 +5434,27 @@
         <v>9</v>
       </c>
       <c r="M32" s="5">
-        <f t="shared" ref="M32:R32" si="12">AVERAGE(M27:M31)</f>
+        <f t="shared" ref="M32:R32" si="14">AVERAGE(M27:M31)</f>
         <v>39.805999999999997</v>
       </c>
       <c r="N32" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10.526</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>29.693999999999999</v>
       </c>
       <c r="P32" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>70.305999999999997</v>
       </c>
       <c r="Q32" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="R32" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5.4</v>
       </c>
       <c r="S32" s="3"/>
@@ -4933,27 +5462,54 @@
         <v>9</v>
       </c>
       <c r="W32" s="5">
-        <f t="shared" ref="W32" si="13">AVERAGE(W27:W31)</f>
+        <f t="shared" ref="W32" si="15">AVERAGE(W27:W31)</f>
         <v>34.254000000000005</v>
       </c>
       <c r="X32" s="5">
-        <f t="shared" ref="X32" si="14">AVERAGE(X27:X31)</f>
+        <f t="shared" ref="X32" si="16">AVERAGE(X27:X31)</f>
         <v>13.652000000000001</v>
       </c>
       <c r="Y32" s="5">
-        <f t="shared" ref="Y32" si="15">AVERAGE(Y27:Y31)</f>
+        <f t="shared" ref="Y32" si="17">AVERAGE(Y27:Y31)</f>
         <v>27.101999999999997</v>
       </c>
       <c r="Z32" s="5">
-        <f t="shared" ref="Z32" si="16">AVERAGE(Z27:Z31)</f>
+        <f t="shared" ref="Z32" si="18">AVERAGE(Z27:Z31)</f>
         <v>72.897999999999996</v>
       </c>
       <c r="AA32" s="5">
-        <f t="shared" ref="AA32" si="17">AVERAGE(AA27:AA31)</f>
+        <f t="shared" ref="AA32" si="19">AVERAGE(AA27:AA31)</f>
         <v>1</v>
       </c>
       <c r="AB32" s="5">
-        <f t="shared" ref="AB32" si="18">AVERAGE(AB27:AB31)</f>
+        <f t="shared" ref="AB32" si="20">AVERAGE(AB27:AB31)</f>
+        <v>6.6</v>
+      </c>
+      <c r="AF32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG32" s="5">
+        <f t="shared" ref="AG32:AL32" si="21">AVERAGE(AG27:AG31)</f>
+        <v>34.254000000000005</v>
+      </c>
+      <c r="AH32" s="5">
+        <f t="shared" si="21"/>
+        <v>13.652000000000001</v>
+      </c>
+      <c r="AI32" s="5">
+        <f t="shared" si="21"/>
+        <v>27.101999999999997</v>
+      </c>
+      <c r="AJ32" s="5">
+        <f t="shared" si="21"/>
+        <v>72.897999999999996</v>
+      </c>
+      <c r="AK32" s="5">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AL32" s="5">
+        <f t="shared" si="21"/>
         <v>6.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add denfis 100% recosntruction
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/SaFIN(FRIE)_HFS_Classification_Results.xlsx
+++ b/Experiment_Resulsts/SaFIN(FRIE)_HFS_Classification_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htetnaing/Development/htet_predict_bank_failure/Experiment_Resulsts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_predict_bank_failure\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB6F649-E497-0E4F-8409-0393A3E61F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D9EC5F-0A14-42DE-A536-2E877E934A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32320" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{59BFD352-3181-4B2E-9A02-E25DF6E8A988}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{59BFD352-3181-4B2E-9A02-E25DF6E8A988}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
@@ -730,30 +730,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F6C734-146C-49B9-BE90-0FF3605E587B}">
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="D10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" customWidth="1"/>
+    <col min="17" max="17" width="15.77734375" customWidth="1"/>
+    <col min="18" max="18" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="33" t="s">
         <v>51</v>
       </c>
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -808,7 +808,7 @@
         <v>3105</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" s="32" t="s">
         <v>13</v>
       </c>
@@ -846,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -890,7 +890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -934,7 +934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -978,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -1122,10 +1122,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="35" t="s">
         <v>51</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="E13" s="32" t="s">
         <v>49</v>
@@ -1172,7 +1172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>3048</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" s="32" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>8</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="E22" s="19"/>
       <c r="G22" s="19"/>
@@ -1561,7 +1561,7 @@
       <c r="P22" s="19"/>
       <c r="R22" s="19"/>
     </row>
-    <row r="23" spans="1:18" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="33" t="s">
         <v>51</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B25" s="32" t="s">
         <v>13</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>8</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="33"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32"/>
@@ -1949,13 +1949,13 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="L33" s="33"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
       <c r="R33" s="32"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -1964,7 +1964,7 @@
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:18" s="14" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" s="14" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>30</v>
       </c>
@@ -1975,7 +1975,7 @@
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="1:18" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" s="25" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>3105</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
         <v>13</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E46" s="2">
         <f>AVERAGE(E41:E45)</f>
         <v>83.418000000000006</v>
@@ -2302,7 +2302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>9</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>
@@ -2343,7 +2343,7 @@
       <c r="Q48" s="7"/>
       <c r="R48" s="7"/>
     </row>
-    <row r="49" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="Q49" s="16"/>
       <c r="R49" s="16"/>
     </row>
-    <row r="50" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="Q50" s="14"/>
       <c r="R50" s="14"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>28</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>3048</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
         <v>13</v>
       </c>
@@ -2440,7 +2440,7 @@
       <c r="Q52" s="12"/>
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E58" s="2">
         <f>AVERAGE(E53:E57)</f>
         <v>72.888000000000005</v>
@@ -2711,7 +2711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="16"/>
       <c r="C60" s="16"/>
@@ -2760,7 +2760,7 @@
       <c r="Q60" s="7"/>
       <c r="R60" s="7"/>
     </row>
-    <row r="61" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>26</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
     </row>
-    <row r="62" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>12</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>29</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B64" s="6" t="s">
         <v>13</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="Q64" s="10"/>
       <c r="R64" s="10"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E70" s="24">
         <f>AVERAGE(E65:E69)</f>
         <v>72.873999999999995</v>
@@ -3111,7 +3111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>9</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L72" s="7" t="s">
         <v>9</v>
       </c>
@@ -3155,20 +3155,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D07C55-6007-C646-9152-6264139E81A7}">
   <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC15" sqref="AC15"/>
+    <sheetView tabSelected="1" topLeftCell="U10" workbookViewId="0">
+      <selection activeCell="AH24" sqref="AH24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="11.5" style="37"/>
-    <col min="12" max="12" width="14.83203125" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="37"/>
-    <col min="21" max="21" width="11.5" style="21"/>
-    <col min="30" max="30" width="11.5" style="37"/>
+    <col min="9" max="9" width="11.44140625" style="37"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="37"/>
+    <col min="21" max="21" width="11.44140625" style="21"/>
+    <col min="30" max="30" width="11.44140625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="33" t="s">
         <v>54</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>3624</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B4" s="32" t="s">
         <v>13</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3430,25 +3430,25 @@
         <v>4</v>
       </c>
       <c r="AG5">
-        <v>20.11</v>
+        <v>74.459999999999994</v>
       </c>
       <c r="AH5">
-        <v>5.41</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="AI5">
-        <v>15.04</v>
+        <v>54.2</v>
       </c>
       <c r="AJ5">
-        <v>84.96</v>
+        <v>45.8</v>
       </c>
       <c r="AK5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3516,16 +3516,16 @@
         <v>5</v>
       </c>
       <c r="AG6">
-        <v>22.46</v>
+        <v>17.03</v>
       </c>
       <c r="AH6">
-        <v>4.13</v>
+        <v>5.75</v>
       </c>
       <c r="AI6">
-        <v>16.12</v>
+        <v>13.41</v>
       </c>
       <c r="AJ6">
-        <v>83.88</v>
+        <v>86.59</v>
       </c>
       <c r="AK6">
         <v>1</v>
@@ -3534,7 +3534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3602,25 +3602,25 @@
         <v>6</v>
       </c>
       <c r="AG7">
-        <v>25.36</v>
+        <v>19.75</v>
       </c>
       <c r="AH7">
-        <v>5.88</v>
+        <v>3.11</v>
       </c>
       <c r="AI7">
-        <v>20.23</v>
+        <v>13.82</v>
       </c>
       <c r="AJ7">
-        <v>79.77</v>
+        <v>86.18</v>
       </c>
       <c r="AK7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3688,25 +3688,25 @@
         <v>7</v>
       </c>
       <c r="AG8">
-        <v>18.3</v>
+        <v>20.11</v>
       </c>
       <c r="AH8">
-        <v>5.2</v>
+        <v>2.77</v>
       </c>
       <c r="AI8">
-        <v>13.62</v>
+        <v>13.17</v>
       </c>
       <c r="AJ8">
-        <v>86.38</v>
+        <v>86.83</v>
       </c>
       <c r="AK8">
         <v>1</v>
       </c>
       <c r="AL8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3774,25 +3774,25 @@
         <v>8</v>
       </c>
       <c r="AG9">
-        <v>5.8</v>
+        <v>18.66</v>
       </c>
       <c r="AH9">
-        <v>75.290000000000006</v>
+        <v>3.28</v>
       </c>
       <c r="AI9">
-        <v>44.65</v>
+        <v>13.31</v>
       </c>
       <c r="AJ9">
-        <v>55.35</v>
+        <v>86.69</v>
       </c>
       <c r="AK9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -3879,30 +3879,30 @@
       </c>
       <c r="AG10" s="5">
         <f t="shared" ref="AG10:AL10" si="3">AVERAGE(AG5:AG9)</f>
-        <v>18.405999999999999</v>
+        <v>30.001999999999999</v>
       </c>
       <c r="AH10" s="5">
         <f t="shared" si="3"/>
-        <v>19.181999999999999</v>
+        <v>6.2200000000000006</v>
       </c>
       <c r="AI10" s="5">
         <f t="shared" si="3"/>
-        <v>21.931999999999999</v>
+        <v>21.582000000000001</v>
       </c>
       <c r="AJ10" s="5">
         <f t="shared" si="3"/>
-        <v>78.067999999999998</v>
+        <v>78.417999999999992</v>
       </c>
       <c r="AK10" s="5">
         <f t="shared" si="3"/>
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="AL10" s="5">
         <f t="shared" si="3"/>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -3936,7 +3936,7 @@
       <c r="AK11" s="16"/>
       <c r="AL11" s="16"/>
     </row>
-    <row r="12" spans="1:38" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="33" t="s">
         <v>54</v>
       </c>
@@ -3969,7 +3969,7 @@
       <c r="AK12" s="32"/>
       <c r="AL12" s="32"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="E13" s="32" t="s">
         <v>49</v>
@@ -4016,7 +4016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>3620</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B15" s="32" t="s">
         <v>13</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -4234,25 +4234,25 @@
         <v>4</v>
       </c>
       <c r="AG16">
-        <v>21.49</v>
+        <v>20.95</v>
       </c>
       <c r="AH16">
-        <v>9.42</v>
+        <v>9.5</v>
       </c>
       <c r="AI16">
-        <v>16.940000000000001</v>
+        <v>16.489999999999998</v>
       </c>
       <c r="AJ16">
-        <v>83.06</v>
+        <v>83.51</v>
       </c>
       <c r="AK16">
         <v>2</v>
       </c>
       <c r="AL16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -4323,25 +4323,25 @@
         <v>5</v>
       </c>
       <c r="AG17">
-        <v>22.63</v>
+        <v>22.81</v>
       </c>
       <c r="AH17">
-        <v>11.41</v>
+        <v>5.28</v>
       </c>
       <c r="AI17">
-        <v>20.07</v>
+        <v>16.79</v>
       </c>
       <c r="AJ17">
-        <v>79.930000000000007</v>
+        <v>83.21</v>
       </c>
       <c r="AK17">
         <v>1</v>
       </c>
       <c r="AL17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -4412,25 +4412,25 @@
         <v>6</v>
       </c>
       <c r="AG18">
-        <v>24.95</v>
+        <v>22.77</v>
       </c>
       <c r="AH18">
-        <v>10.23</v>
+        <v>6.09</v>
       </c>
       <c r="AI18">
-        <v>19.36</v>
+        <v>16.21</v>
       </c>
       <c r="AJ18">
-        <v>80.64</v>
+        <v>83.79</v>
       </c>
       <c r="AK18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -4501,25 +4501,25 @@
         <v>7</v>
       </c>
       <c r="AG19">
-        <v>23.86</v>
+        <v>22.77</v>
       </c>
       <c r="AH19">
-        <v>10.65</v>
+        <v>8.86</v>
       </c>
       <c r="AI19">
-        <v>19.88</v>
+        <v>17.420000000000002</v>
       </c>
       <c r="AJ19">
-        <v>80.12</v>
+        <v>82.58</v>
       </c>
       <c r="AK19">
         <v>1</v>
       </c>
       <c r="AL19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>8</v>
       </c>
@@ -4591,25 +4591,25 @@
         <v>8</v>
       </c>
       <c r="AG20" s="21">
-        <v>24.04</v>
+        <v>22.59</v>
       </c>
       <c r="AH20" s="21">
-        <v>11.25</v>
+        <v>5.45</v>
       </c>
       <c r="AI20" s="21">
-        <v>20.22</v>
+        <v>16.21</v>
       </c>
       <c r="AJ20" s="21">
-        <v>79.78</v>
+        <v>83.79</v>
       </c>
       <c r="AK20" s="21">
         <v>1</v>
       </c>
       <c r="AL20" s="21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
@@ -4700,30 +4700,30 @@
       </c>
       <c r="AG21" s="5">
         <f t="shared" ref="AG21:AL21" si="12">AVERAGE(AG16:AG20)</f>
-        <v>23.393999999999998</v>
+        <v>22.378</v>
       </c>
       <c r="AH21" s="5">
         <f t="shared" si="12"/>
-        <v>10.592000000000001</v>
+        <v>7.0359999999999996</v>
       </c>
       <c r="AI21" s="5">
         <f t="shared" si="12"/>
-        <v>19.294</v>
+        <v>16.624000000000002</v>
       </c>
       <c r="AJ21" s="5">
         <f t="shared" si="12"/>
-        <v>80.705999999999989</v>
+        <v>83.376000000000005</v>
       </c>
       <c r="AK21" s="5">
         <f t="shared" si="12"/>
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="AL21" s="5">
         <f t="shared" si="12"/>
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="E22" s="19"/>
       <c r="G22" s="19"/>
@@ -4742,7 +4742,7 @@
       <c r="AJ22" s="19"/>
       <c r="AL22" s="19"/>
     </row>
-    <row r="23" spans="1:38" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="33" t="s">
         <v>54</v>
       </c>
@@ -4786,7 +4786,7 @@
       <c r="AK23" s="16"/>
       <c r="AL23" s="16"/>
     </row>
-    <row r="24" spans="1:38" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B25" s="32" t="s">
         <v>13</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>3604</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -5056,25 +5056,25 @@
         <v>4</v>
       </c>
       <c r="AG27">
-        <v>28.36</v>
+        <v>25</v>
       </c>
       <c r="AH27">
-        <v>17.21</v>
+        <v>6.73</v>
       </c>
       <c r="AI27">
-        <v>23.58</v>
+        <v>18.84</v>
       </c>
       <c r="AJ27">
-        <v>76.42</v>
+        <v>81.16</v>
       </c>
       <c r="AK27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -5142,25 +5142,25 @@
         <v>5</v>
       </c>
       <c r="AG28">
-        <v>31.34</v>
+        <v>27.05</v>
       </c>
       <c r="AH28">
-        <v>11.55</v>
+        <v>6.35</v>
       </c>
       <c r="AI28">
-        <v>25.09</v>
+        <v>19.96</v>
       </c>
       <c r="AJ28">
-        <v>74.91</v>
+        <v>80.040000000000006</v>
       </c>
       <c r="AK28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -5228,25 +5228,25 @@
         <v>6</v>
       </c>
       <c r="AG29">
-        <v>31.34</v>
+        <v>29.29</v>
       </c>
       <c r="AH29">
-        <v>10.14</v>
+        <v>5.45</v>
       </c>
       <c r="AI29">
-        <v>25.22</v>
+        <v>22.16</v>
       </c>
       <c r="AJ29">
-        <v>74.78</v>
+        <v>77.84</v>
       </c>
       <c r="AK29">
         <v>1</v>
       </c>
       <c r="AL29">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>8</v>
       </c>
@@ -5314,16 +5314,16 @@
         <v>7</v>
       </c>
       <c r="AG30">
-        <v>36.01</v>
+        <v>25.37</v>
       </c>
       <c r="AH30">
-        <v>10.44</v>
+        <v>10.48</v>
       </c>
       <c r="AI30">
-        <v>28.45</v>
+        <v>19.78</v>
       </c>
       <c r="AJ30">
-        <v>71.55</v>
+        <v>80.22</v>
       </c>
       <c r="AK30">
         <v>1</v>
@@ -5332,7 +5332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
@@ -5407,25 +5407,25 @@
         <v>8</v>
       </c>
       <c r="AG31" s="21">
-        <v>44.22</v>
+        <v>28.73</v>
       </c>
       <c r="AH31" s="21">
-        <v>18.920000000000002</v>
+        <v>5.62</v>
       </c>
       <c r="AI31" s="21">
-        <v>33.17</v>
+        <v>21.46</v>
       </c>
       <c r="AJ31" s="21">
-        <v>66.83</v>
+        <v>78.540000000000006</v>
       </c>
       <c r="AK31" s="21">
         <v>1</v>
       </c>
       <c r="AL31" s="21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" ht="21" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="33"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32"/>
@@ -5490,27 +5490,27 @@
       </c>
       <c r="AG32" s="5">
         <f t="shared" ref="AG32:AL32" si="21">AVERAGE(AG27:AG31)</f>
-        <v>34.254000000000005</v>
+        <v>27.088000000000001</v>
       </c>
       <c r="AH32" s="5">
         <f t="shared" si="21"/>
-        <v>13.652000000000001</v>
+        <v>6.9260000000000002</v>
       </c>
       <c r="AI32" s="5">
         <f t="shared" si="21"/>
-        <v>27.101999999999997</v>
+        <v>20.439999999999998</v>
       </c>
       <c r="AJ32" s="5">
         <f t="shared" si="21"/>
-        <v>72.897999999999996</v>
+        <v>79.56</v>
       </c>
       <c r="AK32" s="5">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="AL32" s="5">
         <f t="shared" si="21"/>
-        <v>6.6</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -5522,23 +5522,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBC2BF5-CA36-4037-80F7-043C0B98B69C}">
   <dimension ref="A1:AE54"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -5624,7 +5624,7 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B11">
         <f t="shared" ref="B11:G11" si="0">AVERAGE(B6:B10)</f>
         <v>17.184000000000001</v>
@@ -6079,7 +6079,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -6108,10 +6108,10 @@
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
     </row>
-    <row r="13" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:31" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="AE14" s="15"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -6200,7 +6200,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="21"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
@@ -6259,7 +6259,7 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E23" s="24">
         <f>AVERAGE(E18:E22)</f>
         <v>88.426000000000016</v>
@@ -6622,7 +6622,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>9</v>
       </c>
@@ -6655,10 +6655,10 @@
       <c r="Y24" s="21"/>
       <c r="Z24" s="21"/>
     </row>
-    <row r="25" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E25" s="17"/>
     </row>
-    <row r="28" spans="1:26" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="M28" s="15"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -6701,7 +6701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>3604</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -6758,7 +6758,7 @@
       <c r="V31" s="23"/>
       <c r="W31" s="23"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
         <v>13</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -7074,7 +7074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -7139,7 +7139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E38" s="2">
         <f>AVERAGE(E33:E37)</f>
         <v>79.33</v>
@@ -7177,7 +7177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>9</v>
       </c>
@@ -7206,57 +7206,57 @@
       <c r="V39" s="7"/>
       <c r="W39" s="7"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>43</v>
       </c>

</xml_diff>